<commit_message>
update: figures and code problem update with oaklnad
</commit_message>
<xml_diff>
--- a/added_data/all_cities_restrictions.xlsx
+++ b/added_data/all_cities_restrictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/birth_shotspotter/added_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE274032-BA4D-814D-A73C-8ABD2876AE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B81786F-11C9-E54B-9A9C-FC41F8B1390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{9EFD09F9-5409-9D4F-BB54-7D0921D72F40}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{9EFD09F9-5409-9D4F-BB54-7D0921D72F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,7 +507,7 @@
         <v>42186</v>
       </c>
       <c r="C4" s="2">
-        <v>43313</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>